<commit_message>
renamed all cluspro results
</commit_message>
<xml_diff>
--- a/Project3/scoring.xlsx
+++ b/Project3/scoring.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreyruffolo/Documents/Mizzou/CMP_SC 8170/projects/CS8170-Project1/Project3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4E8D4D-B0A1-BC43-BDA9-3C3181658807}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4F872F-EB7B-C74D-832D-273ED5B0EDB3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="74560" yWindow="10480" windowWidth="21600" windowHeight="18960" xr2:uid="{BD773720-2A0A-B249-97F4-586AD22CB3A1}"/>
+    <workbookView xWindow="74540" yWindow="10500" windowWidth="21600" windowHeight="18960" xr2:uid="{BD773720-2A0A-B249-97F4-586AD22CB3A1}"/>
   </bookViews>
   <sheets>
     <sheet name="ZDock" sheetId="1" r:id="rId1"/>
+    <sheet name="ClusPro" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Target</t>
   </si>
@@ -530,7 +531,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1801,4 +1802,229 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7008AF-3FDF-1E4D-90BC-D6E5AD4A4542}">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>